<commit_message>
Updating calculations, sensors page and adding micro page
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\FlightComputer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39C9D92-6C52-4259-B180-A83F18B12676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A22995-41AD-4859-8345-C96275F01928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4695" yWindow="0" windowWidth="28800" windowHeight="15345" xr2:uid="{9B805F8B-34DA-4B52-9817-F33E613B7037}"/>
   </bookViews>
@@ -525,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A09D79F-AC7F-4CAF-8DBA-6264554563DA}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +583,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>110000</v>
+        <v>130000</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -594,7 +594,7 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>11000</v>
+        <v>12000</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -606,7 +606,7 @@
       </c>
       <c r="B7">
         <f>B4*(B6/(B6+B5))</f>
-        <v>1.3090909090909091</v>
+        <v>1.2169014084507042</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -792,8 +792,7 @@
         <v>24</v>
       </c>
       <c r="B27">
-        <f>4.2*4</f>
-        <v>16.8</v>
+        <v>14.4</v>
       </c>
       <c r="C27" t="s">
         <v>3</v>
@@ -832,7 +831,7 @@
       </c>
       <c r="B31">
         <f>B27*(B30/(B30+B29))</f>
-        <v>2.9443298969072162</v>
+        <v>2.5237113402061855</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -875,7 +874,7 @@
       </c>
       <c r="C36">
         <f>(B27-C34)/C35</f>
-        <v>1.4800000000000001E-2</v>
+        <v>1.24E-2</v>
       </c>
       <c r="D36" t="s">
         <v>22</v>

</xml_diff>